<commit_message>
Fixed component rotations in CPL file for teensy 4.1 12-12 arena with vreg.
</commit_message>
<xml_diff>
--- a/development/arena_12-12_w_vreg/teensy4p1/teensy_arena_12-12_v0p2/production/version_0p2_r1/CPL_JLCPCB_teensy_arena_12-12_v0p2_r1.xlsx
+++ b/development/arena_12-12_w_vreg/teensy4p1/teensy_arena_12-12_v0p2/production/version_0p2_r1/CPL_JLCPCB_teensy_arena_12-12_v0p2_r1.xlsx
@@ -458,7 +458,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +469,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFF6F9D4"/>
       </patternFill>
     </fill>
   </fills>
@@ -513,7 +531,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +560,30 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,6 +593,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFF6F9D4"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFD8CE"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -561,8 +663,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E91" activeCellId="0" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1614,21 +1716,21 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+    <row r="62" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="7" t="n">
         <v>272.1009</v>
       </c>
-      <c r="C62" s="2" t="n">
+      <c r="C62" s="7" t="n">
         <v>-112.8014</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>180</v>
+      <c r="D62" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,293 +2175,293 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+    <row r="89" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="2" t="n">
+      <c r="B89" s="9" t="n">
         <v>285.201</v>
       </c>
-      <c r="C89" s="2" t="n">
+      <c r="C89" s="9" t="n">
         <v>-181.9095</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E89" s="2" t="n">
+      <c r="D89" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="9" t="n">
+        <v>284.1252</v>
+      </c>
+      <c r="C90" s="9" t="n">
+        <v>-232.4759</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="9" t="n">
+        <v>214.3086</v>
+      </c>
+      <c r="C91" s="9" t="n">
+        <v>-284.0016</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="9" t="n">
+        <v>166.55</v>
+      </c>
+      <c r="C92" s="9" t="n">
+        <v>-284.204</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="9" t="n">
+        <v>119.1051</v>
+      </c>
+      <c r="C93" s="9" t="n">
+        <v>-283.391</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="11" t="n">
+        <v>281.6494</v>
+      </c>
+      <c r="C94" s="11" t="n">
+        <v>-158.5468</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="11" t="n">
         <v>-90</v>
       </c>
     </row>
-    <row r="90" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="2" t="n">
-        <v>284.1252</v>
-      </c>
-      <c r="C90" s="2" t="n">
-        <v>-232.4759</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="91" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B91" s="2" t="n">
-        <v>214.3086</v>
-      </c>
-      <c r="C91" s="2" t="n">
-        <v>-284.0016</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="2" t="n">
+    <row r="95" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="11" t="n">
+        <v>258.1096</v>
+      </c>
+      <c r="C95" s="11" t="n">
+        <v>-109.2015</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="11" t="n">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="96" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="11" t="n">
+        <v>213.0509</v>
+      </c>
+      <c r="C96" s="11" t="n">
+        <v>-78.2372</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="11" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="97" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="11" t="n">
+        <v>158.5468</v>
+      </c>
+      <c r="C97" s="11" t="n">
+        <v>-73.9506</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" s="11" t="n">
+        <v>109.2015</v>
+      </c>
+      <c r="C98" s="11" t="n">
+        <v>-97.4904</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="11" t="n">
+        <v>78.2372</v>
+      </c>
+      <c r="C99" s="11" t="n">
+        <v>-142.5491</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="11" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="11" t="n">
+        <v>73.9506</v>
+      </c>
+      <c r="C100" s="11" t="n">
+        <v>-197.0532</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="11" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="11" t="n">
+        <v>97.4904</v>
+      </c>
+      <c r="C101" s="11" t="n">
+        <v>-246.3985</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="11" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="11" t="n">
+        <v>142.5491</v>
+      </c>
+      <c r="C102" s="11" t="n">
+        <v>-277.3628</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="11" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B103" s="11" t="n">
+        <v>197.0532</v>
+      </c>
+      <c r="C103" s="11" t="n">
+        <v>-281.6494</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="11" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="92" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="2" t="n">
-        <v>166.55</v>
-      </c>
-      <c r="C92" s="2" t="n">
-        <v>-284.204</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="93" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B93" s="2" t="n">
-        <v>119.1051</v>
-      </c>
-      <c r="C93" s="2" t="n">
-        <v>-283.391</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="94" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="2" t="n">
-        <v>281.6494</v>
-      </c>
-      <c r="C94" s="2" t="n">
-        <v>-158.5468</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B95" s="2" t="n">
-        <v>258.1096</v>
-      </c>
-      <c r="C95" s="2" t="n">
-        <v>-109.2015</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="96" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B96" s="2" t="n">
-        <v>213.0509</v>
-      </c>
-      <c r="C96" s="2" t="n">
-        <v>-78.2372</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="97" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B97" s="2" t="n">
-        <v>158.5468</v>
-      </c>
-      <c r="C97" s="2" t="n">
-        <v>-73.9506</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="98" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B98" s="2" t="n">
-        <v>109.2015</v>
-      </c>
-      <c r="C98" s="2" t="n">
-        <v>-97.4904</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="99" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B99" s="2" t="n">
-        <v>78.2372</v>
-      </c>
-      <c r="C99" s="2" t="n">
-        <v>-142.5491</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="100" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="2" t="n">
-        <v>73.9506</v>
-      </c>
-      <c r="C100" s="2" t="n">
-        <v>-197.0532</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="101" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B101" s="2" t="n">
-        <v>97.4904</v>
-      </c>
-      <c r="C101" s="2" t="n">
-        <v>-246.3985</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="2" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="102" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B102" s="2" t="n">
-        <v>142.5491</v>
-      </c>
-      <c r="C102" s="2" t="n">
-        <v>-277.3628</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="103" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B103" s="2" t="n">
-        <v>197.0532</v>
-      </c>
-      <c r="C103" s="2" t="n">
-        <v>-281.6494</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="2" t="n">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="104" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
+    <row r="104" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="2" t="n">
+      <c r="B104" s="11" t="n">
         <v>246.3985</v>
       </c>
-      <c r="C104" s="2" t="n">
+      <c r="C104" s="11" t="n">
         <v>-258.1096</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="105" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="s">
+      <c r="D104" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="11" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="105" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B105" s="2" t="n">
+      <c r="B105" s="11" t="n">
         <v>277.3628</v>
       </c>
-      <c r="C105" s="2" t="n">
+      <c r="C105" s="11" t="n">
         <v>-213.0509</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="2" t="n">
-        <v>-30</v>
+      <c r="D105" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="11" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="106" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>